<commit_message>
corrected the appliances analysis for yearwise and for all. also removed extra navigation bar from dashboard
</commit_message>
<xml_diff>
--- a/server/data/energy_dashboard_final_data_corrected.xlsx
+++ b/server/data/energy_dashboard_final_data_corrected.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jigya\OneDrive\Desktop\bebu\green-energy-main\server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEA0990-5411-4B4D-80FE-857880FB0017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD8D90E-4CCA-4C8F-82D5-3F6EB0E06673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,7 +567,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>34715.937456703818</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -614,10 +614,10 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>25215.433807411591</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>29061.904106408241</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -628,10 +628,10 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>10609.902742089749</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>4295.629165596667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>